<commit_message>
List of transceiver modules
</commit_message>
<xml_diff>
--- a/Amateur Radio Repeater/Transceiver Modules.xlsx
+++ b/Amateur Radio Repeater/Transceiver Modules.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Transceiver module</t>
   </si>
@@ -84,6 +84,33 @@
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/2244900.pdf</t>
+  </si>
+  <si>
+    <t>TH71221</t>
+  </si>
+  <si>
+    <t>Melexis</t>
+  </si>
+  <si>
+    <t>27-930MHz</t>
+  </si>
+  <si>
+    <t>+10dBm</t>
+  </si>
+  <si>
+    <t>38.6mA*5.5V=212.3mW</t>
+  </si>
+  <si>
+    <t>Cant find it</t>
+  </si>
+  <si>
+    <t>115 kbps</t>
+  </si>
+  <si>
+    <t>-107 dBm</t>
+  </si>
+  <si>
+    <t>https://www.melexis.com/-/media/files/documents/datasheets/th71221-datasheet-melexis.pdf</t>
   </si>
 </sst>
 </file>
@@ -413,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,6 +524,38 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1"/>

</xml_diff>